<commit_message>
add parser for szigetmonostor
</commit_message>
<xml_diff>
--- a/data_source.xlsx
+++ b/data_source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\QM\data\osm\gimmisn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E62FB42-7816-475F-A0F3-24E02947F77F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE50D46F-7AA6-4DF4-88F8-3270979344C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="215">
   <si>
     <t>Típus</t>
   </si>
@@ -672,6 +672,12 @@
   </si>
   <si>
     <t>Sződliget</t>
+  </si>
+  <si>
+    <t>szigetmonostor.hu</t>
+  </si>
+  <si>
+    <t>nincs újabb 2020.08.23</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,11 +4078,20 @@
       <c r="B153" t="s">
         <v>13</v>
       </c>
-      <c r="C153" t="s">
-        <v>52</v>
+      <c r="C153" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D153">
+        <v>2015</v>
       </c>
       <c r="E153" t="s">
         <v>82</v>
+      </c>
+      <c r="F153" s="6">
+        <v>43615</v>
+      </c>
+      <c r="G153" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -4757,8 +4772,9 @@
     <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="C40" r:id="rId4" xr:uid="{9C118C4B-DF81-4CD3-9047-2DCC66C9E141}"/>
+    <hyperlink ref="C153" r:id="rId5" xr:uid="{4F65A167-0AEF-4FFC-9103-CD88761D6EA9}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId5"/>
+  <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>